<commit_message>
Wizualizacja dodawania i edytowania tras
</commit_message>
<xml_diff>
--- a/Baza_nasza.xlsx
+++ b/Baza_nasza.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\Documents\GitHub\SWD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studia\Semestr 5\Systemy Wspomagania Decyzji\Projekt\SWD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2D4332-4A90-4222-893B-7B323E1BF77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67ED952-B015-4E41-9493-3DB77BCB6380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{797E9F96-CA76-4F4F-B032-5C734006C564}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{797E9F96-CA76-4F4F-B032-5C734006C564}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -128,9 +129,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -168,7 +169,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -274,7 +275,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -416,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -424,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69BF0FF-2BD0-41DC-80B1-E8D4EC5F42E3}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +445,7 @@
     <col min="10" max="10" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,14 +464,8 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1500</v>
       </c>
@@ -481,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <f>A2/IF(F2 = "Pieszo", $I$2, IF(F2 = "Narty", $I$3, IF(F2 = "Skuter", $I$4, $I$5)))*(B2/10+1)*(C2/20+1) + IF(F2 = "Pieszo", $J$2, IF(F2 = "Narty", $J$3, IF(F2 = "Skuter", $J$4, $J$5)))</f>
+        <f>A2/IF(F2 = "Pieszo", Arkusz2!$B$2, IF(F2 = "Narty", Arkusz2!$B$3, IF(F2 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B2/10+1)*(C2/20+1) + IF(F2 = "Pieszo", Arkusz2!$C$2, IF(F2 = "Narty", Arkusz2!$C$3, IF(F2 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>6.3857228554289147</v>
       </c>
       <c r="E2">
@@ -490,17 +485,8 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2">
-        <v>84</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1500</v>
       </c>
@@ -512,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">A3/IF(F3 = "Pieszo", $I$2, IF(F3 = "Narty", $I$3, IF(F3 = "Skuter", $I$4, $I$5)))*(B3/10+1)*(C3/20+1) + IF(F3 = "Pieszo", $J$2, IF(F3 = "Narty", $J$3, IF(F3 = "Skuter", $J$4, $J$5)))</f>
+        <f>A3/IF(F3 = "Pieszo", Arkusz2!$B$2, IF(F3 = "Narty", Arkusz2!$B$3, IF(F3 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B3/10+1)*(C3/20+1) + IF(F3 = "Pieszo", Arkusz2!$C$2, IF(F3 = "Narty", Arkusz2!$C$3, IF(F3 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>6.08</v>
       </c>
       <c r="E3">
@@ -521,17 +507,8 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3">
-        <v>750</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1500</v>
       </c>
@@ -543,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>A4/IF(F4 = "Pieszo", Arkusz2!$B$2, IF(F4 = "Narty", Arkusz2!$B$3, IF(F4 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B4/10+1)*(C4/20+1) + IF(F4 = "Pieszo", Arkusz2!$C$2, IF(F4 = "Narty", Arkusz2!$C$3, IF(F4 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>27.500000000000004</v>
       </c>
       <c r="E4">
@@ -552,17 +529,8 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>1667</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3000</v>
       </c>
@@ -573,7 +541,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>A5/IF(F5 = "Pieszo", Arkusz2!$B$2, IF(F5 = "Narty", Arkusz2!$B$3, IF(F5 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B5/10+1)*(C5/20+1) + IF(F5 = "Pieszo", Arkusz2!$C$2, IF(F5 = "Narty", Arkusz2!$C$3, IF(F5 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>7.8074385122975407</v>
       </c>
       <c r="E5">
@@ -582,17 +550,8 @@
       <c r="F5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5">
-        <v>4167</v>
-      </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3000</v>
       </c>
@@ -603,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f>A6/IF(F6 = "Pieszo", Arkusz2!$B$2, IF(F6 = "Narty", Arkusz2!$B$3, IF(F6 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B6/10+1)*(C6/20+1) + IF(F6 = "Pieszo", Arkusz2!$C$2, IF(F6 = "Narty", Arkusz2!$C$3, IF(F6 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>9.24</v>
       </c>
       <c r="E6">
@@ -613,7 +572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3000</v>
       </c>
@@ -624,7 +583,7 @@
         <v>4</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f>A7/IF(F7 = "Pieszo", Arkusz2!$B$2, IF(F7 = "Narty", Arkusz2!$B$3, IF(F7 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B7/10+1)*(C7/20+1) + IF(F7 = "Pieszo", Arkusz2!$C$2, IF(F7 = "Narty", Arkusz2!$C$3, IF(F7 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>55.714285714285715</v>
       </c>
       <c r="E7">
@@ -634,7 +593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4800</v>
       </c>
@@ -645,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f>A8/IF(F8 = "Pieszo", Arkusz2!$B$2, IF(F8 = "Narty", Arkusz2!$B$3, IF(F8 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B8/10+1)*(C8/20+1) + IF(F8 = "Pieszo", Arkusz2!$C$2, IF(F8 = "Narty", Arkusz2!$C$3, IF(F8 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>9.9670065986802641</v>
       </c>
       <c r="E8">
@@ -655,7 +614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4800</v>
       </c>
@@ -666,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f>A9/IF(F9 = "Pieszo", Arkusz2!$B$2, IF(F9 = "Narty", Arkusz2!$B$3, IF(F9 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B9/10+1)*(C9/20+1) + IF(F9 = "Pieszo", Arkusz2!$C$2, IF(F9 = "Narty", Arkusz2!$C$3, IF(F9 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>14.520000000000001</v>
       </c>
       <c r="E9">
@@ -676,7 +635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4800</v>
       </c>
@@ -687,7 +646,7 @@
         <v>5</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f>A10/IF(F10 = "Pieszo", Arkusz2!$B$2, IF(F10 = "Narty", Arkusz2!$B$3, IF(F10 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B10/10+1)*(C10/20+1) + IF(F10 = "Pieszo", Arkusz2!$C$2, IF(F10 = "Narty", Arkusz2!$C$3, IF(F10 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>107.14285714285715</v>
       </c>
       <c r="E10">
@@ -697,7 +656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -708,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>A11/IF(F11 = "Pieszo", Arkusz2!$B$2, IF(F11 = "Narty", Arkusz2!$B$3, IF(F11 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B11/10+1)*(C11/20+1) + IF(F11 = "Pieszo", Arkusz2!$C$2, IF(F11 = "Narty", Arkusz2!$C$3, IF(F11 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
         <v>10.275977921766259</v>
       </c>
       <c r="E11">
@@ -716,6 +675,77 @@
       </c>
       <c r="F11" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A0C0D3-1AB0-4580-B587-2E93FE7582EC}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>84</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>750</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1667</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>4167</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodanie punktów odniesienia i wag
</commit_message>
<xml_diff>
--- a/Baza_nasza.xlsx
+++ b/Baza_nasza.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studia\Semestr 5\Systemy Wspomagania Decyzji\Projekt\SWD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\Documents\GitHub\SWD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67ED952-B015-4E41-9493-3DB77BCB6380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51E9F50-B500-46FC-ACAE-9BFAC65F39A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{797E9F96-CA76-4F4F-B032-5C734006C564}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{797E9F96-CA76-4F4F-B032-5C734006C564}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office 2013–2022">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +169,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office 2013–2022">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -275,7 +275,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office 2013–2022">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -428,7 +428,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,14 +661,14 @@
         <v>1000</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11">
         <f>A11/IF(F11 = "Pieszo", Arkusz2!$B$2, IF(F11 = "Narty", Arkusz2!$B$3, IF(F11 = "Skuter", Arkusz2!$B$4, Arkusz2!$B$5)))*(B11/10+1)*(C11/20+1) + IF(F11 = "Pieszo", Arkusz2!$C$2, IF(F11 = "Narty", Arkusz2!$C$3, IF(F11 = "Skuter", Arkusz2!$C$4, Arkusz2!$C$5)))</f>
-        <v>10.275977921766259</v>
+        <v>10.303575713942884</v>
       </c>
       <c r="E11">
         <v>0</v>

</xml_diff>